<commit_message>
handling multi value types
</commit_message>
<xml_diff>
--- a/tests/data/dms-unknown-value-type.xlsx
+++ b/tests/data/dms-unknown-value-type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08168CF2-1F4A-462B-A3DC-9CB1A77070F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74844360-A6D3-944A-8EE6-34A262948C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="16780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
   <si>
     <t>role</t>
   </si>
@@ -167,6 +167,15 @@
   </si>
   <si>
     <t>In Model</t>
+  </si>
+  <si>
+    <t>cable</t>
+  </si>
+  <si>
+    <t>operator</t>
+  </si>
+  <si>
+    <t>creationTime</t>
   </si>
 </sst>
 </file>
@@ -188,16 +197,19 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="20"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -561,13 +573,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -583,7 +595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -591,7 +603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -599,7 +611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -607,12 +619,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -620,7 +632,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -628,7 +640,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -636,7 +648,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -644,7 +656,7 @@
         <v>45414.735154691647</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -652,7 +664,7 @@
         <v>45414.735154691647</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -667,25 +679,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.5" customWidth="1"/>
     <col min="2" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="14.44140625" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="14.5" customWidth="1"/>
+    <col min="12" max="12" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5" customWidth="1"/>
     <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
@@ -705,7 +717,7 @@
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
     </row>
-    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -755,7 +767,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -791,7 +803,7 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -827,7 +839,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>31</v>
       </c>
@@ -863,7 +875,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
@@ -898,6 +910,114 @@
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -916,14 +1036,14 @@
       <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>37</v>
       </c>
@@ -935,7 +1055,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -961,7 +1081,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -984,19 +1104,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>40</v>
       </c>
@@ -1006,7 +1126,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -1026,7 +1146,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Opinionated conversion of value type edge cases (#637)
* handling multi value types

* fix resolution of multi value and uknown types

* added changelog

* improve comment

* fix to anyuri

* fix static typing

* remove print
</commit_message>
<xml_diff>
--- a/tests/data/dms-unknown-value-type.xlsx
+++ b/tests/data/dms-unknown-value-type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08168CF2-1F4A-462B-A3DC-9CB1A77070F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74844360-A6D3-944A-8EE6-34A262948C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="16780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
   <si>
     <t>role</t>
   </si>
@@ -167,6 +167,15 @@
   </si>
   <si>
     <t>In Model</t>
+  </si>
+  <si>
+    <t>cable</t>
+  </si>
+  <si>
+    <t>operator</t>
+  </si>
+  <si>
+    <t>creationTime</t>
   </si>
 </sst>
 </file>
@@ -188,16 +197,19 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="20"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -561,13 +573,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -583,7 +595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -591,7 +603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -599,7 +611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -607,12 +619,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -620,7 +632,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -628,7 +640,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -636,7 +648,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -644,7 +656,7 @@
         <v>45414.735154691647</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -652,7 +664,7 @@
         <v>45414.735154691647</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -667,25 +679,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.5" customWidth="1"/>
     <col min="2" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="14.44140625" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="14.5" customWidth="1"/>
+    <col min="12" max="12" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5" customWidth="1"/>
     <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
@@ -705,7 +717,7 @@
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
     </row>
-    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -755,7 +767,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -791,7 +803,7 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -827,7 +839,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>31</v>
       </c>
@@ -863,7 +875,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
@@ -898,6 +910,114 @@
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -916,14 +1036,14 @@
       <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>37</v>
       </c>
@@ -935,7 +1055,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -961,7 +1081,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -984,19 +1104,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>40</v>
       </c>
@@ -1006,7 +1126,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -1026,7 +1146,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>

</xml_diff>